<commit_message>
MI emissions small update
</commit_message>
<xml_diff>
--- a/state_fact_sheets/data/modified/mi_emissions_summary.xlsx
+++ b/state_fact_sheets/data/modified/mi_emissions_summary.xlsx
@@ -7629,7 +7629,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -7649,7 +7649,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -7669,7 +7669,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -7689,7 +7689,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -7709,7 +7709,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -7729,7 +7729,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -7749,7 +7749,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -7769,7 +7769,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -7789,7 +7789,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -7809,7 +7809,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -7829,7 +7829,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -7849,7 +7849,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -7869,7 +7869,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -7889,7 +7889,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -7909,7 +7909,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -7929,7 +7929,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -7949,7 +7949,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -7969,7 +7969,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -7989,7 +7989,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -8009,7 +8009,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -8029,7 +8029,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -8049,7 +8049,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -8069,7 +8069,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -8089,7 +8089,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -8109,7 +8109,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -8129,7 +8129,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -8149,7 +8149,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -8169,7 +8169,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -8189,7 +8189,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -8209,7 +8209,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -8229,7 +8229,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -8249,7 +8249,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -8269,7 +8269,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>
@@ -8289,7 +8289,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Total</t>
+          <t>Tons CO2 eq</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
MI emissions summary update
</commit_message>
<xml_diff>
--- a/state_fact_sheets/data/modified/mi_emissions_summary.xlsx
+++ b/state_fact_sheets/data/modified/mi_emissions_summary.xlsx
@@ -8,7 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Emissions by Unit" sheetId="1" r:id="rId1"/>
-    <sheet name="Emissions by Facility and Fuel" sheetId="2" r:id="rId2"/>
+    <sheet name="Emissions by Fclty, Fuel" sheetId="2" r:id="rId2"/>
+    <sheet name="Emissions by Fclty, Fuel, GHG" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -8656,4 +8657,2259 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D115"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>facility_name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>fuel_type</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>ghg_name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>total_ghg</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Billerud Escanaba LLC</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Bituminous</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D2">
+        <v>851.4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Billerud Escanaba LLC</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Bituminous</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D3">
+        <v>2.3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Billerud Escanaba LLC</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Bituminous</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Billerud Escanaba LLC</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D5">
+        <v>308726.2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Billerud Escanaba LLC</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D6">
+        <v>145.5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Billerud Escanaba LLC</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D7">
+        <v>173.4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Billerud Escanaba LLC</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Propane</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D8">
+        <v>18.1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Billerud Escanaba LLC</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Propane</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Billerud Escanaba LLC</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Propane</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Billerud Escanaba LLC</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Tires</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Billerud Escanaba LLC</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Tires</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Billerud Escanaba LLC</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Tires</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Billerud Escanaba LLC</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Wood and Wood Residuals (dry basis)</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D14">
+        <v>485496.5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Billerud Escanaba LLC</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Wood and Wood Residuals (dry basis)</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D15">
+        <v>931.6999999999999</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Billerud Escanaba LLC</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Wood and Wood Residuals (dry basis)</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D16">
+        <v>5552.7</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Billerud Escanaba LLC</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Biogenic (Spent Liquor)</t>
+        </is>
+      </c>
+      <c r="D17">
+        <v>1108645.4</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Billerud Escanaba LLC</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Non-Biogenic</t>
+        </is>
+      </c>
+      <c r="D18">
+        <v>25657.5</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Billerud Escanaba LLC</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Methane</t>
+        </is>
+      </c>
+      <c r="D19">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Billerud Escanaba LLC</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Methane Spent Liquor</t>
+        </is>
+      </c>
+      <c r="D20">
+        <v>22.32</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Billerud Escanaba LLC</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide</t>
+        </is>
+      </c>
+      <c r="D21">
+        <v>0.123</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Billerud Escanaba LLC</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide Spent Liquor</t>
+        </is>
+      </c>
+      <c r="D22">
+        <v>4.932</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Billerud Quinnesec LLC</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Bituminous</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Billerud Quinnesec LLC</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Bituminous</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Billerud Quinnesec LLC</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Bituminous</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D25">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Billerud Quinnesec LLC</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D26">
+        <v>22754.6</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Billerud Quinnesec LLC</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D27">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Billerud Quinnesec LLC</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D28">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Billerud Quinnesec LLC</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Propane</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D29">
+        <v>27.1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Billerud Quinnesec LLC</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Propane</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Billerud Quinnesec LLC</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Propane</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D31">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Billerud Quinnesec LLC</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Wood and Wood Residuals (dry basis)</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Billerud Quinnesec LLC</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Wood and Wood Residuals (dry basis)</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D33">
+        <v>686.6</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Billerud Quinnesec LLC</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Wood and Wood Residuals (dry basis)</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D34">
+        <v>4092.1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Billerud Quinnesec LLC</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Biogenic (Spent Liquor)</t>
+        </is>
+      </c>
+      <c r="D35">
+        <v>630900.7</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Billerud Quinnesec LLC</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Non-Biogenic</t>
+        </is>
+      </c>
+      <c r="D36">
+        <v>41101</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Billerud Quinnesec LLC</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Methane</t>
+        </is>
+      </c>
+      <c r="D37">
+        <v>1.96</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Billerud Quinnesec LLC</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Methane Spent Liquor</t>
+        </is>
+      </c>
+      <c r="D38">
+        <v>12.79</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Billerud Quinnesec LLC</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide</t>
+        </is>
+      </c>
+      <c r="D39">
+        <v>0.008</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Billerud Quinnesec LLC</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide Spent Liquor</t>
+        </is>
+      </c>
+      <c r="D40">
+        <v>2.828</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>CARBON GREEN BIOENERGY</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D41">
+        <v>80502</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>CARBON GREEN BIOENERGY</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D42">
+        <v>37.9</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>CARBON GREEN BIOENERGY</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D43">
+        <v>45.2</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>CARBON GREEN BIOENERGY</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Other Biomass Gases</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D44">
+        <v>197.4</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>CARBON GREEN BIOENERGY</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Other Biomass Gases</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D45">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>CARBON GREEN BIOENERGY</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Other Biomass Gases</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D46">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>CARGILL SALT SAINT CLAIR</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D47">
+        <v>97911</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>CARGILL SALT SAINT CLAIR</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D48">
+        <v>46.1</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>CARGILL SALT SAINT CLAIR</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D49">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Cargill Salt</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D50">
+        <v>40109</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Cargill Salt</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D51">
+        <v>18.9</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Cargill Salt</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D52">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>MARYSVILLE ETHANOL LLC</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D53">
+        <v>83851.39999999999</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>MARYSVILLE ETHANOL LLC</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D54">
+        <v>39.5</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>MARYSVILLE ETHANOL LLC</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D55">
+        <v>47.09999999999999</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR CO - CARO FACTORY</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Anthracite</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D56">
+        <v>3059.5</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR CO - CARO FACTORY</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Anthracite</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D57">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR CO - CARO FACTORY</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Anthracite</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D58">
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR CO - CARO FACTORY</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Coal Coke</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D59">
+        <v>2255.2</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR CO - CARO FACTORY</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Coal Coke</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D60">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR CO - CARO FACTORY</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Coal Coke</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D61">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR CO - CARO FACTORY</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D62">
+        <v>48923.1</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR CO - CARO FACTORY</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D63">
+        <v>23.1</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR CO - CARO FACTORY</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D64">
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR CO - CROSWELL FACTORY</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D65">
+        <v>59782.39999999999</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR CO - CROSWELL FACTORY</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D66">
+        <v>28.1</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR CO - CROSWELL FACTORY</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D67">
+        <v>33.5</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR COMPANY - Bay City</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Anthracite</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D68">
+        <v>5616.8</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR COMPANY - Bay City</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Anthracite</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D69">
+        <v>14.9</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR COMPANY - Bay City</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Anthracite</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D70">
+        <v>25.8</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR COMPANY - Bay City</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Coal Coke</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D71">
+        <v>8738.9</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR COMPANY - Bay City</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Coal Coke</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D72">
+        <v>21.1</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR COMPANY - Bay City</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Coal Coke</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D73">
+        <v>36.7</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR COMPANY - Bay City</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D74">
+        <v>115986.6</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR COMPANY - Bay City</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D75">
+        <v>54.59999999999999</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR COMPANY - Bay City</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D76">
+        <v>65.2</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR COMPANY - SEBEWAING FACTORY</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Anthracite</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D77">
+        <v>6004.5</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR COMPANY - SEBEWAING FACTORY</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Anthracite</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D78">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR COMPANY - SEBEWAING FACTORY</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Anthracite</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D79">
+        <v>27.6</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR COMPANY - SEBEWAING FACTORY</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Bituminous</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D80">
+        <v>68866.5</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR COMPANY - SEBEWAING FACTORY</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Bituminous</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D81">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR COMPANY - SEBEWAING FACTORY</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Bituminous</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D82">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR COMPANY - SEBEWAING FACTORY</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D83">
+        <v>29082.9</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR COMPANY - SEBEWAING FACTORY</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D84">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>MICHIGAN SUGAR COMPANY - SEBEWAING FACTORY</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D85">
+        <v>16.4</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>MORTON SALT</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Bituminous</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D86">
+        <v>92584.7</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>MORTON SALT</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Bituminous</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D87">
+        <v>272.9</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>MORTON SALT</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Bituminous</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D88">
+        <v>473.2</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>MORTON SALT</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D89">
+        <v>1435.7</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>MORTON SALT</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D90">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>MORTON SALT</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D91">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>NEENAH PAPER MICHIGAN INC</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Bituminous</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D92">
+        <v>44563.2</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>NEENAH PAPER MICHIGAN INC</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Bituminous</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D93">
+        <v>131.4</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>NEENAH PAPER MICHIGAN INC</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Bituminous</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D94">
+        <v>227.8</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>NEENAH PAPER MICHIGAN INC</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Distillate Fuel Oil No. 2</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>NEENAH PAPER MICHIGAN INC</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Distillate Fuel Oil No. 2</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>NEENAH PAPER MICHIGAN INC</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Distillate Fuel Oil No. 2</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>NEENAH PAPER MICHIGAN INC</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D98">
+        <v>23286.9</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>NEENAH PAPER MICHIGAN INC</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D99">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>NEENAH PAPER MICHIGAN INC</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D100">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Otsego Paper, Inc.</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D101">
+        <v>111236.5</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Otsego Paper, Inc.</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D102">
+        <v>52.4</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Otsego Paper, Inc.</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D103">
+        <v>62.40000000000001</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>POET Biorefining - Caro, LLC</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D104">
+        <v>105694.8</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>POET Biorefining - Caro, LLC</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D105">
+        <v>49.8</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>POET Biorefining - Caro, LLC</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D106">
+        <v>59.4</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>THE ANDERSONS MARATHON HOLDINGS LLC</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D107">
+        <v>206644.9</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>THE ANDERSONS MARATHON HOLDINGS LLC</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D108">
+        <v>97.40000000000001</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>THE ANDERSONS MARATHON HOLDINGS LLC</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D109">
+        <v>116.1</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>UP Paper LLC</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D110">
+        <v>52081.3</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>UP Paper LLC</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D111">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>UP Paper LLC</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Natural Gas (Weighted U.S. Average)</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D112">
+        <v>29.3</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>UP Paper LLC</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Natural Gasoline</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Carbon Dioxide Total</t>
+        </is>
+      </c>
+      <c r="D113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>UP Paper LLC</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Natural Gasoline</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Methane (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>UP Paper LLC</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Natural Gasoline</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Nitrous Oxide (Co2 eq)</t>
+        </is>
+      </c>
+      <c r="D115">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>